<commit_message>
first attempt in multiple linear regression model
</commit_message>
<xml_diff>
--- a/resources/genealogy_matrix.xlsx
+++ b/resources/genealogy_matrix.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t xml:space="preserve">Focal Name</t>
   </si>
@@ -205,7 +206,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -597,101 +598,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="1" t="n">
-        <v>0</v>
-      </c>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
@@ -822,4 +763,476 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>7124</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>